<commit_message>
cg: update cg forms
</commit_message>
<xml_diff>
--- a/ONCHO/OEM/Congo/2023/cg_oncho_oem_202303_2_biopsie.xlsx
+++ b/ONCHO/OEM/Congo/2023/cg_oncho_oem_202303_2_biopsie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\ONCHO\OEM\Congo\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EECEF02-186E-4642-BB75-27E504B70CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE9B7AF-2B6A-47FF-9E30-450AED77DB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="186">
   <si>
     <t>type</t>
   </si>
@@ -510,12 +510,6 @@
     <t>French</t>
   </si>
   <si>
-    <t>cg_oncho_oem_202303_2_biopsie</t>
-  </si>
-  <si>
-    <t>(2023 Mars) CEO - 2 Formulaire Biopsie</t>
-  </si>
-  <si>
     <t>Cuvette Ouest</t>
   </si>
   <si>
@@ -574,6 +568,18 @@
   </si>
   <si>
     <t>Sembé-Souaké</t>
+  </si>
+  <si>
+    <t>cg_oncho_oem_202303_2_biopsiev_2</t>
+  </si>
+  <si>
+    <t>(2023 Mars) CEO - 2 Formulaire Biopsie V2</t>
+  </si>
+  <si>
+    <t>Le DBS a-t-il été prélevé?</t>
+  </si>
+  <si>
+    <t>dbs_preleve</t>
   </si>
 </sst>
 </file>
@@ -993,13 +999,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23:G23"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1523,32 +1529,34 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" t="s">
-        <v>87</v>
-      </c>
+    <row r="24" spans="1:13" s="3" customFormat="1">
+      <c r="A24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D24" s="13"/>
       <c r="H24" s="13" t="s">
         <v>57</v>
       </c>
+      <c r="I24"/>
       <c r="J24" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H25" s="13" t="s">
         <v>57</v>
@@ -1557,18 +1565,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="31.5">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="J26" s="13" t="s">
         <v>19</v>
@@ -1576,13 +1584,13 @@
     </row>
     <row r="27" spans="1:13" ht="31.5">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>92</v>
@@ -1591,43 +1599,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="3" customFormat="1">
-      <c r="A28" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="G28" s="13"/>
+    <row r="28" spans="1:13" ht="31.5">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>95</v>
+      </c>
       <c r="H28" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="I28" s="13"/>
+        <v>92</v>
+      </c>
       <c r="J28" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" ht="15.75" customHeight="1">
+    </row>
+    <row r="29" spans="1:13" s="3" customFormat="1">
       <c r="A29" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>100</v>
+      <c r="B29" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13" t="s">
         <v>57</v>
@@ -1640,47 +1640,72 @@
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
     </row>
-    <row r="30" spans="1:13">
-      <c r="A30" t="s">
+    <row r="30" spans="1:13" s="3" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
         <v>42</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>101</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>102</v>
       </c>
-      <c r="J30" s="13"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="3" t="s">
+      <c r="J31" s="13"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H31" s="13"/>
-      <c r="J31" s="13"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="3"/>
       <c r="H32" s="13"/>
       <c r="J32" s="13"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" t="s">
-        <v>104</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="H33" s="13"/>
       <c r="J33" s="13"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="s">
+        <v>104</v>
+      </c>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
         <v>105</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>105</v>
       </c>
-      <c r="J34" s="13"/>
+      <c r="J35" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2109,10 +2134,10 @@
         <v>107</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="11"/>
@@ -2122,10 +2147,10 @@
         <v>107</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="11"/>
@@ -2135,10 +2160,10 @@
         <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="11"/>
@@ -2161,10 +2186,10 @@
         <v>107</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="11"/>
@@ -2187,10 +2212,10 @@
         <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="11"/>
@@ -2281,13 +2306,13 @@
         <v>142</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E45" s="11"/>
     </row>
@@ -2296,13 +2321,13 @@
         <v>142</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E46" s="11"/>
     </row>
@@ -2311,13 +2336,13 @@
         <v>142</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E47" s="11"/>
     </row>
@@ -2326,13 +2351,13 @@
         <v>142</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E48" s="11"/>
     </row>
@@ -2341,13 +2366,13 @@
         <v>142</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E49" s="11"/>
     </row>
@@ -2362,7 +2387,7 @@
         <v>148</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E50" s="11"/>
     </row>
@@ -2377,7 +2402,7 @@
         <v>149</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E51" s="11"/>
     </row>
@@ -2416,10 +2441,10 @@
         <v>142</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>140</v>
@@ -2461,13 +2486,13 @@
         <v>142</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E57" s="11"/>
     </row>
@@ -2476,13 +2501,13 @@
         <v>142</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E58" s="11"/>
     </row>
@@ -2491,13 +2516,13 @@
         <v>142</v>
       </c>
       <c r="B59" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C59" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D59" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2505,13 +2530,13 @@
         <v>142</v>
       </c>
       <c r="B60" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C60" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D60" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2533,10 +2558,10 @@
         <v>142</v>
       </c>
       <c r="B62" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C62" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D62" t="s">
         <v>141</v>
@@ -2575,10 +2600,10 @@
         <v>142</v>
       </c>
       <c r="B65" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C65" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D65" t="s">
         <v>141</v>
@@ -2603,10 +2628,10 @@
         <v>142</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C67" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D67" t="s">
         <v>141</v>
@@ -2617,13 +2642,13 @@
         <v>142</v>
       </c>
       <c r="B68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D68" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2631,13 +2656,13 @@
         <v>142</v>
       </c>
       <c r="B69" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C69" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D69" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2651,7 +2676,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2673,10 +2698,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
         <v>161</v>

</xml_diff>